<commit_message>
Updates to bring Metadata tab syntax closer in line with TTL.
":" introduced for default namespace.
":data" replaces @data-namespace
":schema" replaces @schema-namespace
</commit_message>
<xml_diff>
--- a/src/test/resources/test11.xlsx
+++ b/src/test/resources/test11.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Loader" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Humans" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Purchases" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Info" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Loader" sheetId="1" r:id="rId1"/>
+    <sheet name="Humans" sheetId="2" r:id="rId2"/>
+    <sheet name="Purchases" sheetId="3" r:id="rId3"/>
+    <sheet name="Info" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Sheet Name</t>
   </si>
@@ -119,15 +118,9 @@
     <t>http://sales.data/purchases/2015</t>
   </si>
   <si>
-    <t>@data-namespace</t>
-  </si>
-  <si>
     <t>http://sales.data/purchases#</t>
   </si>
   <si>
-    <t>@schema-namespace</t>
-  </si>
-  <si>
     <t>http://sales.data/schema#</t>
   </si>
   <si>
@@ -159,38 +152,25 @@
   </si>
   <si>
     <t># Row 8 is a comment</t>
+  </si>
+  <si>
+    <t>:data</t>
+  </si>
+  <si>
+    <t>:schema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -209,7 +189,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -217,176 +197,420 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="D1:D3 A12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" activeCellId="1" sqref="D1:D3 A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="19.7109375"/>
+    <col min="2" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="D1:D3 D10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" activeCellId="1" sqref="D1:D3 D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.85425101214575"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="5.85546875"/>
+    <col min="2" max="2" width="13.140625"/>
+    <col min="3" max="3" width="11.42578125"/>
+    <col min="4" max="4" width="12.140625"/>
+    <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -403,7 +627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -411,7 +635,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>18</v>
@@ -426,43 +650,35 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="D1:D3 A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" activeCellId="1" sqref="D1:D3 A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.71255060728745"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="11.140625"/>
+    <col min="2" max="2" width="12.7109375"/>
+    <col min="3" max="4" width="8.5703125"/>
+    <col min="5" max="5" width="9.7109375"/>
+    <col min="6" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -482,7 +698,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -491,7 +707,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -504,51 +720,43 @@
       <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="6">
         <v>41952</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="34.28515625"/>
+    <col min="3" max="3" width="37.28515625"/>
+    <col min="4" max="4" width="39.140625"/>
+    <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -561,77 +769,78 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="7" t="s">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7" t="s">
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>46</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>